<commit_message>
update with BOM import function
</commit_message>
<xml_diff>
--- a/plm-database.xlsx
+++ b/plm-database.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Items" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BOM-001" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BOM-002" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -36,7 +35,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -47,6 +46,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="001a4d2e"/>
         <bgColor rgb="001a4d2e"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00f0f0f0"/>
+        <bgColor rgb="00f0f0f0"/>
       </patternFill>
     </fill>
     <fill>
@@ -68,7 +73,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -76,7 +81,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -442,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,11 +461,11 @@
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="30" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
-    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
     <col width="18" customWidth="1" min="9" max="9"/>
     <col width="18" customWidth="1" min="10" max="10"/>
     <col width="18" customWidth="1" min="11" max="11"/>
@@ -470,6 +478,7 @@
     <col width="18" customWidth="1" min="18" max="18"/>
     <col width="18" customWidth="1" min="19" max="19"/>
     <col width="18" customWidth="1" min="20" max="20"/>
+    <col width="18" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -490,85 +499,95 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>REVISION</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>STATUS</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>CATEGORY</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>DESCRIPTION</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>UoM</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>MANUFACTURER_1</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>MANUFACTURER_CODE_1</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>MANUFACTURER_2</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>MANUFACTURER_CODE_2</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>SUPPLIER_1</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>SUPPLIER_CODE_1</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>SUPPLIER_COST_1</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>SUPPLIER_2</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>SUPPLIER_CODE_2</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>SUPPLIER_COST_2</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>SUPPLIER_3</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>SUPPLIER_CODE_3</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>SUPPLIER_COST_3</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>COST</t>
         </is>
@@ -587,90 +606,100 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>GB001</t>
+          <t>GB0001</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
           <t>Electronics</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Resistor 100K Ohm 1/4W</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="H2" s="2" t="inlineStr">
         <is>
           <t>pcs</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>Yageo</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="J2" s="2" t="inlineStr">
         <is>
           <t>RC0805FR-07100KL</t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="K2" s="2" t="inlineStr">
         <is>
           <t>Vishay</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="L2" s="2" t="inlineStr">
         <is>
           <t>CRCW0805100KFKEA</t>
         </is>
       </c>
-      <c r="K2" s="2" t="inlineStr">
+      <c r="M2" s="2" t="inlineStr">
         <is>
           <t>Mouser</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
+      <c r="N2" s="2" t="inlineStr">
         <is>
           <t>603-RC0805FR-07100KL</t>
         </is>
       </c>
-      <c r="M2" s="2" t="inlineStr">
+      <c r="O2" s="2" t="inlineStr">
         <is>
           <t>0.05</t>
         </is>
       </c>
-      <c r="N2" s="2" t="inlineStr">
+      <c r="P2" s="2" t="inlineStr">
         <is>
           <t>Digikey</t>
         </is>
       </c>
-      <c r="O2" s="2" t="inlineStr">
+      <c r="Q2" s="2" t="inlineStr">
         <is>
           <t>311-100KCRCT-ND</t>
         </is>
       </c>
-      <c r="P2" s="2" t="inlineStr">
+      <c r="R2" s="2" t="inlineStr">
         <is>
           <t>0.06</t>
         </is>
       </c>
-      <c r="Q2" s="2" t="inlineStr">
+      <c r="S2" s="2" t="inlineStr">
         <is>
           <t>Arrow</t>
         </is>
       </c>
-      <c r="R2" s="2" t="inlineStr">
+      <c r="T2" s="2" t="inlineStr">
         <is>
           <t>71-CRCW0805-100K-E3</t>
         </is>
       </c>
-      <c r="S2" s="2" t="inlineStr">
+      <c r="U2" s="2" t="inlineStr">
         <is>
           <t>0.05</t>
         </is>
       </c>
-      <c r="T2" s="2" t="inlineStr">
+      <c r="V2" s="2" t="inlineStr">
         <is>
           <t>0.05</t>
         </is>
@@ -689,90 +718,100 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>GB002</t>
+          <t>GB0002</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
           <t>Electronics</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="G3" s="2" t="inlineStr">
         <is>
           <t>Capacitor 10uF 25V Ceramic</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="H3" s="2" t="inlineStr">
         <is>
           <t>pcs</t>
         </is>
       </c>
-      <c r="G3" s="2" t="inlineStr">
+      <c r="I3" s="2" t="inlineStr">
         <is>
           <t>Murata</t>
         </is>
       </c>
-      <c r="H3" s="2" t="inlineStr">
+      <c r="J3" s="2" t="inlineStr">
         <is>
           <t>GRM21BR61E106KA73L</t>
         </is>
       </c>
-      <c r="I3" s="2" t="inlineStr">
+      <c r="K3" s="2" t="inlineStr">
         <is>
           <t>Samsung</t>
         </is>
       </c>
-      <c r="J3" s="2" t="inlineStr">
+      <c r="L3" s="2" t="inlineStr">
         <is>
           <t>CL21A106KAYNNNE</t>
         </is>
       </c>
-      <c r="K3" s="2" t="inlineStr">
+      <c r="M3" s="2" t="inlineStr">
         <is>
           <t>Mouser</t>
         </is>
       </c>
-      <c r="L3" s="2" t="inlineStr">
+      <c r="N3" s="2" t="inlineStr">
         <is>
           <t>81-GRM21BR61E106KA3L</t>
         </is>
       </c>
-      <c r="M3" s="2" t="inlineStr">
+      <c r="O3" s="2" t="inlineStr">
         <is>
           <t>0.15</t>
         </is>
       </c>
-      <c r="N3" s="2" t="inlineStr">
+      <c r="P3" s="2" t="inlineStr">
         <is>
           <t>Digikey</t>
         </is>
       </c>
-      <c r="O3" s="2" t="inlineStr">
+      <c r="Q3" s="2" t="inlineStr">
         <is>
           <t>490-3886-1-ND</t>
         </is>
       </c>
-      <c r="P3" s="2" t="inlineStr">
+      <c r="R3" s="2" t="inlineStr">
         <is>
           <t>0.16</t>
         </is>
       </c>
-      <c r="Q3" s="2" t="inlineStr">
+      <c r="S3" s="2" t="inlineStr">
         <is>
           <t>LCSC</t>
         </is>
       </c>
-      <c r="R3" s="2" t="inlineStr">
+      <c r="T3" s="2" t="inlineStr">
         <is>
           <t>C15850</t>
         </is>
       </c>
-      <c r="S3" s="2" t="inlineStr">
+      <c r="U3" s="2" t="inlineStr">
         <is>
           <t>0.12</t>
         </is>
       </c>
-      <c r="T3" s="2" t="inlineStr">
+      <c r="V3" s="2" t="inlineStr">
         <is>
           <t>0.15</t>
         </is>
@@ -791,72 +830,162 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>GB003</t>
+          <t>GB0003</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
           <t>Hardware</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
+      <c r="G4" s="2" t="inlineStr">
         <is>
           <t>Screw M3x10mm Stainless Steel</t>
         </is>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="H4" s="2" t="inlineStr">
         <is>
           <t>pcs</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr">
+      <c r="I4" s="2" t="inlineStr">
         <is>
           <t>McMaster</t>
         </is>
       </c>
-      <c r="H4" s="2" t="inlineStr">
+      <c r="J4" s="2" t="inlineStr">
         <is>
           <t>92005A120</t>
         </is>
       </c>
-      <c r="I4" s="2" t="inlineStr"/>
-      <c r="J4" s="2" t="inlineStr"/>
-      <c r="K4" s="2" t="inlineStr">
+      <c r="K4" s="2" t="inlineStr"/>
+      <c r="L4" s="2" t="inlineStr"/>
+      <c r="M4" s="2" t="inlineStr">
         <is>
           <t>McMaster</t>
         </is>
       </c>
-      <c r="L4" s="2" t="inlineStr">
+      <c r="N4" s="2" t="inlineStr">
         <is>
           <t>92005A120</t>
         </is>
       </c>
-      <c r="M4" s="2" t="inlineStr">
+      <c r="O4" s="2" t="inlineStr">
         <is>
           <t>0.10</t>
         </is>
       </c>
-      <c r="N4" s="2" t="inlineStr">
+      <c r="P4" s="2" t="inlineStr">
         <is>
           <t>Fastenal</t>
         </is>
       </c>
-      <c r="O4" s="2" t="inlineStr">
+      <c r="Q4" s="2" t="inlineStr">
         <is>
           <t>11282765</t>
         </is>
       </c>
-      <c r="P4" s="2" t="inlineStr">
+      <c r="R4" s="2" t="inlineStr">
         <is>
           <t>0.12</t>
         </is>
       </c>
-      <c r="Q4" s="2" t="inlineStr"/>
-      <c r="R4" s="2" t="inlineStr"/>
       <c r="S4" s="2" t="inlineStr"/>
-      <c r="T4" s="2" t="inlineStr">
+      <c r="T4" s="2" t="inlineStr"/>
+      <c r="U4" s="2" t="inlineStr"/>
+      <c r="V4" s="2" t="inlineStr">
         <is>
           <t>0.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>RES-100K</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>10001</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>GB0004</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>A0</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>Obsolete</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>Resistor 100K Ohm 1/4W (old revision)</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>Yageo</t>
+        </is>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>RC0805FR-07100KL-OLD</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="inlineStr"/>
+      <c r="L5" s="3" t="inlineStr"/>
+      <c r="M5" s="3" t="inlineStr">
+        <is>
+          <t>Mouser</t>
+        </is>
+      </c>
+      <c r="N5" s="3" t="inlineStr">
+        <is>
+          <t>603-RC0805FR-OLD</t>
+        </is>
+      </c>
+      <c r="O5" s="3" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="P5" s="3" t="inlineStr"/>
+      <c r="Q5" s="3" t="inlineStr"/>
+      <c r="R5" s="3" t="inlineStr"/>
+      <c r="S5" s="3" t="inlineStr"/>
+      <c r="T5" s="3" t="inlineStr"/>
+      <c r="U5" s="3" t="inlineStr"/>
+      <c r="V5" s="3" t="inlineStr">
+        <is>
+          <t>0.06</t>
         </is>
       </c>
     </row>
@@ -871,7 +1000,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -886,7 +1015,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>BOMCODE</t>
         </is>
@@ -898,7 +1027,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>DESCRIPTION</t>
         </is>
@@ -910,7 +1039,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>CREATED_DATE</t>
         </is>
@@ -922,7 +1051,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
@@ -933,230 +1062,103 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>REVISION</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>ALIAS</t>
         </is>
       </c>
-      <c r="B6" s="1" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>GBCODE</t>
         </is>
       </c>
-      <c r="C6" s="1" t="inlineStr">
+      <c r="C7" s="1" t="inlineStr">
         <is>
           <t>QUANTITY</t>
         </is>
       </c>
-      <c r="D6" s="1" t="inlineStr">
+      <c r="D7" s="1" t="inlineStr">
         <is>
           <t>NOTES</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>RES-100K</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>GB001</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>Pull-up resistors</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>CAP-10UF</t>
+          <t>RES-100K</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>GB002</t>
+          <t>GB0001</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>Power supply decoupling</t>
+          <t>Pull-up resistors</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
+          <t>CAP-10UF</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>GB0002</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>Power supply decoupling</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
           <t>SCR-M3X10</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>GB003</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>GB0003</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="D9" s="2" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>Panel mounting screws</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="30" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>BOMCODE</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>BOM-002</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>DESCRIPTION</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Power Supply Module</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>CREATED_DATE</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2024-01-20</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>STATUS</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Draft</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>ALIAS</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>GBCODE</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>QUANTITY</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="inlineStr">
-        <is>
-          <t>NOTES</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>CAP-10UF</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>GB002</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>Output filtering</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>RES-100K</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>GB001</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>Feedback network</t>
         </is>
       </c>
     </row>

</xml_diff>